<commit_message>
modify efficient net function
</commit_message>
<xml_diff>
--- a/project/submissions/results.xlsx
+++ b/project/submissions/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentroduit/Documents/document_vincent/epfl/master/ma2/image_analysis/EE-451-IAPR/project/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C88A24B-D0AC-5940-8A12-CEE6C63B05BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C426B50A-505F-9544-8217-B760217CAECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" xr2:uid="{30B75F18-E009-2F48-96FD-76C3DE01CBCF}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="12">
   <si>
     <t>Image Size</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Efficient Net</t>
   </si>
 </sst>
 </file>
@@ -910,10 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2905451-230E-F94E-978F-0BFE8AA12A7C}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -959,53 +965,53 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
       <c r="E3">
-        <v>0.6804</v>
+        <v>0.72199999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E4">
-        <v>0.62419999999999998</v>
+        <v>0.77410000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5">
-        <v>0.72199999999999998</v>
+        <v>0.6804</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1013,16 +1019,16 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
       <c r="E6">
-        <v>0.8216</v>
+        <v>0.62419999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1047,16 +1053,84 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>300</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>0.76880000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C8">
+      <c r="C9">
+        <v>300</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>0.8216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
         <v>400</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D10" t="s">
         <v>5</v>
       </c>
-      <c r="E8">
+      <c r="E10">
         <v>0.80110000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>300</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>0.84150000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>300</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>0.98650000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added files and augmentaion viz
</commit_message>
<xml_diff>
--- a/project/submissions/results.xlsx
+++ b/project/submissions/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentroduit/Documents/document_vincent/epfl/master/ma2/image_analysis/EE-451-IAPR/project/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF743957-D462-0243-A908-73690019E9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2AE76C-113B-4148-9E7E-4BF48006E9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" xr2:uid="{30B75F18-E009-2F48-96FD-76C3DE01CBCF}"/>
   </bookViews>
@@ -919,7 +919,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E12"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>